<commit_message>
DataProvider aplicacion de pagos
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataAplicacionPagoPagaduria.xlsx
+++ b/src/test/resources/Data/AutomationDataAplicacionPagoPagaduria.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5884A5E-B26B-4EE6-BB80-5E862D08AF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8ABD0A-247B-4680-9722-1C562C55CAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CarguePlanillaAlSistema" sheetId="10" r:id="rId1"/>
-    <sheet name="PreaplicacionPagaduria" sheetId="12" r:id="rId2"/>
-    <sheet name="AplicacionFinalPagaduria" sheetId="13" r:id="rId3"/>
+    <sheet name="AplicacionPago" sheetId="10" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Periodo</t>
   </si>
@@ -47,34 +45,31 @@
     <t>RutaPagaduria</t>
   </si>
   <si>
-    <t>CUERPO OFICIAL DE BOMBEROS BOGOTA</t>
-  </si>
-  <si>
     <t>"C:\\Users\\User\\Downloads\\PlanillasCarguePagaduria\\"</t>
   </si>
   <si>
-    <t>Pagaduria</t>
-  </si>
-  <si>
     <t>IdPagaduria</t>
   </si>
   <si>
     <t>Ano</t>
   </si>
   <si>
-    <t>"CUERPO OFICIAL DE BOMBEROS BOGOTA"</t>
-  </si>
-  <si>
-    <t>"2021"</t>
-  </si>
-  <si>
     <t>Octubre 30</t>
   </si>
   <si>
+    <t>30/10/2021</t>
+  </si>
+  <si>
+    <t>PeriodoEspacio</t>
+  </si>
+  <si>
+    <t>FiltroFecha</t>
+  </si>
+  <si>
+    <t>"BANCO DE LA REPUBLICA NOMINA JUBILADOS"</t>
+  </si>
+  <si>
     <t>"Octubre  30"</t>
-  </si>
-  <si>
-    <t>30/10/2021</t>
   </si>
 </sst>
 </file>
@@ -400,37 +395,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>271</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+      <c r="E2" s="2">
+        <v>2021</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -438,79 +459,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AF64ED-BAEB-4A00-AB30-12BCAC7FDD09}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF13A82C-9101-4B23-80B9-484E3EF5980F}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajuste Archivo Cargue Pagaduria
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataAplicacionPagoPagaduria.xlsx
+++ b/src/test/resources/Data/AutomationDataAplicacionPagoPagaduria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8ABD0A-247B-4680-9722-1C562C55CAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66737101-1EB5-4442-B645-8241430F1E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>RutaPagaduria</t>
   </si>
   <si>
-    <t>"C:\\Users\\User\\Downloads\\PlanillasCarguePagaduria\\"</t>
-  </si>
-  <si>
     <t>IdPagaduria</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>"Octubre  30"</t>
+  </si>
+  <si>
+    <t>"src/test/resources/Data/PagaduriaAplicacion/"</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +410,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -422,13 +422,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -436,22 +436,22 @@
         <v>271</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2">
         <v>2021</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste validación amortización X Naturaleza de cuentas
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataAplicacionPagoPagaduria.xlsx
+++ b/src/test/resources/Data/AutomationDataAplicacionPagoPagaduria.xlsx
@@ -1,40 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F6D260-A80B-470C-AABA-700CF7E43729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4056D803-8371-4EEB-A3C7-B80A17845CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AplicacionPago" sheetId="10" r:id="rId1"/>
+    <sheet name="AplicacionPago" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>IdPagaduria</t>
+  </si>
   <si>
     <t>Periodo</t>
   </si>
@@ -45,68 +39,62 @@
     <t>RutaPagaduria</t>
   </si>
   <si>
-    <t>IdPagaduria</t>
-  </si>
-  <si>
     <t>Ano</t>
   </si>
   <si>
-    <t>Octubre 30</t>
-  </si>
-  <si>
-    <t>30/10/2021</t>
-  </si>
-  <si>
     <t>PeriodoEspacio</t>
   </si>
   <si>
     <t>FiltroFecha</t>
   </si>
   <si>
-    <t>"BANCO DE LA REPUBLICA NOMINA JUBILADOS"</t>
-  </si>
-  <si>
-    <t>"Octubre  30"</t>
+    <t>AccountingSource</t>
+  </si>
+  <si>
+    <t>AccountingName</t>
+  </si>
+  <si>
+    <t>FechaRegistro</t>
+  </si>
+  <si>
+    <t>Noviembre 30</t>
   </si>
   <si>
     <t>"src/test/resources/Data/PagaduriaAplicacion/"</t>
   </si>
   <si>
-    <t>AccountingSource</t>
-  </si>
-  <si>
-    <t>AccountingName</t>
-  </si>
-  <si>
-    <t>FechaRegistro</t>
+    <t>"Noviembre  30"</t>
+  </si>
+  <si>
+    <t>30/11/2021</t>
   </si>
   <si>
     <t>"'APLPAG'"</t>
   </si>
   <si>
-    <t>"upper('Aplicación de pago por pagaduría')"</t>
-  </si>
-  <si>
-    <t>25/11/2021</t>
+    <t>"upper('Aplicación de pago por pagaduría'),  upper('Aplicación de pago venta en firme') "</t>
+  </si>
+  <si>
+    <t>10/12/2021</t>
+  </si>
+  <si>
+    <t>"CONSORCIO DE PENSIONES DEL HUILA"</t>
+  </si>
+  <si>
+    <t>103</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,11 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,7 +138,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -168,7 +154,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -180,7 +166,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -197,7 +183,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -227,12 +213,29 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -262,6 +265,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,87 +433,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>271</v>
+      <c r="A2" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>2021</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ejecución y ajuste flujo de aplicación de pagos - 10 Pagadurias
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataAplicacionPagoPagaduria.xlsx
+++ b/src/test/resources/Data/AutomationDataAplicacionPagoPagaduria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4056D803-8371-4EEB-A3C7-B80A17845CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4CEDDA-5C2D-4DD5-BB1D-A5E2633AACEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,13 +75,13 @@
     <t>"upper('Aplicación de pago por pagaduría'),  upper('Aplicación de pago venta en firme') "</t>
   </si>
   <si>
-    <t>10/12/2021</t>
-  </si>
-  <si>
-    <t>"CONSORCIO DE PENSIONES DEL HUILA"</t>
-  </si>
-  <si>
-    <t>103</t>
+    <t>22/12/2021</t>
+  </si>
+  <si>
+    <t>349</t>
+  </si>
+  <si>
+    <t>"ALCALDÍA MUNICIPAL DE BARRANCABERMEJA NÓMINA TRABAJADORES OFICIALES"</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,13 +487,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Creacion Dinamica Contable "Cierre"
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataAplicacionPagoPagaduria.xlsx
+++ b/src/test/resources/Data/AutomationDataAplicacionPagoPagaduria.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4CEDDA-5C2D-4DD5-BB1D-A5E2633AACEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC2D654-B4A4-43D7-9E0F-13D01ADBEA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AplicacionPago" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>IdPagaduria</t>
   </si>
@@ -69,19 +69,34 @@
     <t>30/11/2021</t>
   </si>
   <si>
+    <t>"ALCALDIA MUNICIPAL DE IBAGUE PENSIONADOS"</t>
+  </si>
+  <si>
+    <t>183</t>
+  </si>
+  <si>
+    <t>17/01/2022</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>AccountingSourceCierre</t>
+  </si>
+  <si>
     <t>"'APLPAG'"</t>
   </si>
   <si>
-    <t>"upper('Aplicación de pago por pagaduría'),  upper('Aplicación de pago venta en firme') "</t>
-  </si>
-  <si>
-    <t>22/12/2021</t>
-  </si>
-  <si>
-    <t>349</t>
-  </si>
-  <si>
-    <t>"ALCALDÍA MUNICIPAL DE BARRANCABERMEJA NÓMINA TRABAJADORES OFICIALES"</t>
+    <t>"'CIERRE'"</t>
+  </si>
+  <si>
+    <t>"upper('Aplicación de pago por pagaduría') "</t>
+  </si>
+  <si>
+    <t>"upper('Causación fianza cierre de periodo')"</t>
+  </si>
+  <si>
+    <t>AccountingNameCierre</t>
   </si>
 </sst>
 </file>
@@ -434,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +468,7 @@
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,22 +499,28 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1">
-        <v>2021</v>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>12</v>
@@ -508,13 +529,19 @@
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>